<commit_message>
Completed Data Field Matrix
I entered the second half of the systems from the equipment schedule master.
</commit_message>
<xml_diff>
--- a/ScheduleEntryForms/Documentation/DataFieldMatrix.xlsx
+++ b/ScheduleEntryForms/Documentation/DataFieldMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhanp\source\repos\nhanphan2112\Aire.DataEntryForms\ScheduleEntryForms\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA5A307-A804-4687-849B-AA00477FAA82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CE7FBA-E816-4A97-AF0D-38839B1F610F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B54BB1EA-0F42-48C7-90BB-C62F55C48395}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B54BB1EA-0F42-48C7-90BB-C62F55C48395}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="COLOR CODE" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NhanVersion!$A$1:$I$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NhanVersion!$A$1:$S$72</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AK$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -62,7 +62,11 @@
   <authors>
     <author>tc={EBC03C0B-FBE9-4C04-9B11-228985458680}</author>
     <author>tc={2FF6A1BC-CE4F-4650-8A6B-93878D8AB648}</author>
-    <author>tc={36A4241A-0832-47CB-AAC6-1457863971B4}</author>
+    <author>tc={D488B709-F195-4D5F-97EF-4A96910E96D5}</author>
+    <author>tc={72DA17CC-47E6-4AF2-B923-5B6A79DD819C}</author>
+    <author>tc={955CF92B-6B5E-41FD-AD61-6A0083BBC1A6}</author>
+    <author>tc={17BC0988-34DD-4D6C-9FBF-37DE15D980EC}</author>
+    <author>tc={8659692C-E75B-4676-8180-4523FBF0CB15}</author>
   </authors>
   <commentList>
     <comment ref="H1" authorId="0" shapeId="0" xr:uid="{EBC03C0B-FBE9-4C04-9B11-228985458680}">
@@ -81,12 +85,44 @@
     Outdoor Condensing/Heat Pump Units</t>
       </text>
     </comment>
-    <comment ref="A32" authorId="2" shapeId="0" xr:uid="{36A4241A-0832-47CB-AAC6-1457863971B4}">
+    <comment ref="K1" authorId="2" shapeId="0" xr:uid="{D488B709-F195-4D5F-97EF-4A96910E96D5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    VoltPhase mean either Volt or Phase will be entered because engineer are retards</t>
+    Fan Coil Units</t>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="3" shapeId="0" xr:uid="{72DA17CC-47E6-4AF2-B923-5B6A79DD819C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Also called as MARK in equipment schedule</t>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="4" shapeId="0" xr:uid="{955CF92B-6B5E-41FD-AD61-6A0083BBC1A6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    also called Model HP</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="5" shapeId="0" xr:uid="{17BC0988-34DD-4D6C-9FBF-37DE15D980EC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    also called Model FC</t>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="6" shapeId="0" xr:uid="{8659692C-E75B-4676-8180-4523FBF0CB15}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    also called outdoor unit mark</t>
       </text>
     </comment>
   </commentList>
@@ -94,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
   <si>
     <t>VAV</t>
   </si>
@@ -255,20 +291,134 @@
     <t>VENTING</t>
   </si>
   <si>
-    <t>DO NOT START ISOLATION WO NOAH</t>
-  </si>
-  <si>
     <t>Sone</t>
   </si>
   <si>
-    <t>OHP</t>
+    <t>MINISPLIT HEATPUMPS</t>
+  </si>
+  <si>
+    <t>HeatPumpLocation</t>
+  </si>
+  <si>
+    <t>FanCoilLocation</t>
+  </si>
+  <si>
+    <t>SEER</t>
+  </si>
+  <si>
+    <t>SP_inchwg</t>
+  </si>
+  <si>
+    <t>HeatPumpLWA</t>
+  </si>
+  <si>
+    <t>HeatPumpWeight_lbs</t>
+  </si>
+  <si>
+    <t>AUX_kw</t>
+  </si>
+  <si>
+    <t>IndoorUnitModel</t>
+  </si>
+  <si>
+    <t>OutdoorUnitModel</t>
+  </si>
+  <si>
+    <t>IndoorUnitTag</t>
+  </si>
+  <si>
+    <t>OutdoorUnitTag</t>
+  </si>
+  <si>
+    <t>OHP -  HEAT PUMP UNITS</t>
+  </si>
+  <si>
+    <t>IHP - FAN COIL UNITS</t>
+  </si>
+  <si>
+    <t>GAS FURNACE</t>
+  </si>
+  <si>
+    <t>AFUE</t>
+  </si>
+  <si>
+    <t>NumberOfStages</t>
+  </si>
+  <si>
+    <t>InputMBH</t>
+  </si>
+  <si>
+    <t>OutputMBH</t>
+  </si>
+  <si>
+    <t>GASRTU - GAS FIRED ROOFTOP UNIT</t>
+  </si>
+  <si>
+    <t>HPRTU - HEATPUMP ROOFTOP UNIT</t>
+  </si>
+  <si>
+    <t>GRD - GRILLES, REGISTERS &amp; DEFFUSERS</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Mounting</t>
+  </si>
+  <si>
+    <t>HEATER - ELECTRIC DUCT HEATERS</t>
+  </si>
+  <si>
+    <t>Size_WidthAndLength_inch</t>
+  </si>
+  <si>
+    <t>DeltaT</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>ISOLATION</t>
+  </si>
+  <si>
+    <t>IsolatedEquipment</t>
+  </si>
+  <si>
+    <t>DeflectionPerInch</t>
+  </si>
+  <si>
+    <t>LbsPerIsolator</t>
+  </si>
+  <si>
+    <t>FtOfSoundLinerNeeded</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>LOUVERS/HOODS</t>
+  </si>
+  <si>
+    <t>MaxIntake_fpm</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>VFD - VARIABLE FREQUENCY DRIVE</t>
+  </si>
+  <si>
+    <t>RatedAmps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,12 +490,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -477,7 +621,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -498,8 +642,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="60% - Accent2" xfId="5" builtinId="36"/>
@@ -841,8 +986,20 @@
   <threadedComment ref="I1" dT="2021-02-24T04:26:22.14" personId="{E0428C46-52C3-4581-9E7B-36125533829F}" id="{2FF6A1BC-CE4F-4650-8A6B-93878D8AB648}">
     <text>Outdoor Condensing/Heat Pump Units</text>
   </threadedComment>
-  <threadedComment ref="A32" dT="2021-02-24T03:35:25.83" personId="{E0428C46-52C3-4581-9E7B-36125533829F}" id="{36A4241A-0832-47CB-AAC6-1457863971B4}">
-    <text>VoltPhase mean either Volt or Phase will be entered because engineer are retards</text>
+  <threadedComment ref="K1" dT="2021-02-25T02:56:03.09" personId="{E0428C46-52C3-4581-9E7B-36125533829F}" id="{D488B709-F195-4D5F-97EF-4A96910E96D5}">
+    <text>Fan Coil Units</text>
+  </threadedComment>
+  <threadedComment ref="S2" dT="2021-02-25T04:33:13.67" personId="{E0428C46-52C3-4581-9E7B-36125533829F}" id="{72DA17CC-47E6-4AF2-B923-5B6A79DD819C}">
+    <text>Also called as MARK in equipment schedule</text>
+  </threadedComment>
+  <threadedComment ref="A5" dT="2021-02-25T03:24:55.95" personId="{E0428C46-52C3-4581-9E7B-36125533829F}" id="{955CF92B-6B5E-41FD-AD61-6A0083BBC1A6}">
+    <text>also called Model HP</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2021-02-25T03:25:07.04" personId="{E0428C46-52C3-4581-9E7B-36125533829F}" id="{17BC0988-34DD-4D6C-9FBF-37DE15D980EC}">
+    <text>also called Model FC</text>
+  </threadedComment>
+  <threadedComment ref="A15" dT="2021-02-25T03:19:41.54" personId="{E0428C46-52C3-4581-9E7B-36125533829F}" id="{8659692C-E75B-4676-8180-4523FBF0CB15}">
+    <text>also called outdoor unit mark</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1936,13 +2093,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D3163-F64C-485F-B08A-A467FA0F7EED}">
-  <dimension ref="A1:AB43"/>
+  <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1952,9 +2109,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
-        <v>53</v>
-      </c>
+      <c r="A1" s="12"/>
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1977,18 +2132,38 @@
         <v>52</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="T1" s="20"/>
       <c r="U1" s="20"/>
       <c r="V1" s="20"/>
@@ -2011,16 +2186,16 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
@@ -2043,16 +2218,16 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
       <c r="T3" s="9"/>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
@@ -2075,16 +2250,16 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
       <c r="V4" s="9"/>
@@ -2096,27 +2271,27 @@
       <c r="AB4" s="9"/>
     </row>
     <row r="5" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
-        <v>40</v>
+      <c r="A5" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
       <c r="T5" s="9"/>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
@@ -2128,27 +2303,27 @@
       <c r="AB5" s="9"/>
     </row>
     <row r="6" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
@@ -2161,26 +2336,26 @@
     </row>
     <row r="7" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="11"/>
       <c r="T7" s="9"/>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>
@@ -2193,26 +2368,26 @@
     </row>
     <row r="8" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="10"/>
       <c r="T8" s="9"/>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
@@ -2225,9 +2400,9 @@
     </row>
     <row r="9" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="10"/>
+        <v>55</v>
+      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -2235,16 +2410,16 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
@@ -2257,26 +2432,26 @@
     </row>
     <row r="10" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
@@ -2289,26 +2464,26 @@
     </row>
     <row r="11" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="13" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="11"/>
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
       <c r="V11" s="9"/>
@@ -2321,26 +2496,26 @@
     </row>
     <row r="12" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="13" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="10"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
@@ -2353,26 +2528,26 @@
     </row>
     <row r="13" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="10"/>
       <c r="T13" s="9"/>
       <c r="U13" s="9"/>
       <c r="V13" s="9"/>
@@ -2385,9 +2560,9 @@
     </row>
     <row r="14" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -2395,16 +2570,16 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
@@ -2417,26 +2592,26 @@
     </row>
     <row r="15" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="13" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="10"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
@@ -2449,26 +2624,26 @@
     </row>
     <row r="16" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="13" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
@@ -2481,26 +2656,26 @@
     </row>
     <row r="17" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="13" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
@@ -2513,26 +2688,26 @@
     </row>
     <row r="18" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
@@ -2545,26 +2720,26 @@
     </row>
     <row r="19" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A19" s="13" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="11"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
       <c r="T19" s="9"/>
       <c r="U19" s="9"/>
       <c r="V19" s="9"/>
@@ -2576,27 +2751,27 @@
       <c r="AB19" s="9"/>
     </row>
     <row r="20" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="16" t="s">
-        <v>28</v>
+      <c r="A20" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="10"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
       <c r="V20" s="9"/>
@@ -2608,27 +2783,27 @@
       <c r="AB20" s="9"/>
     </row>
     <row r="21" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="16" t="s">
-        <v>29</v>
+      <c r="A21" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
       <c r="T21" s="9"/>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
@@ -2640,27 +2815,27 @@
       <c r="AB21" s="9"/>
     </row>
     <row r="22" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="10"/>
+      <c r="A22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
@@ -2672,27 +2847,27 @@
       <c r="AB22" s="9"/>
     </row>
     <row r="23" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="11"/>
+      <c r="A23" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
       <c r="T23" s="9"/>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
@@ -2704,27 +2879,27 @@
       <c r="AB23" s="9"/>
     </row>
     <row r="24" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="15" t="s">
-        <v>31</v>
+      <c r="A24" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="B24" s="11"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
       <c r="V24" s="9"/>
@@ -2736,27 +2911,27 @@
       <c r="AB24" s="9"/>
     </row>
     <row r="25" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="21" t="s">
-        <v>51</v>
+      <c r="A25" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
       <c r="T25" s="9"/>
       <c r="U25" s="9"/>
       <c r="V25" s="9"/>
@@ -2769,26 +2944,26 @@
     </row>
     <row r="26" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
       <c r="T26" s="9"/>
       <c r="U26" s="9"/>
       <c r="V26" s="9"/>
@@ -2801,9 +2976,9 @@
     </row>
     <row r="27" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="10"/>
+        <v>90</v>
+      </c>
+      <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -2811,16 +2986,16 @@
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="11"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
@@ -2833,9 +3008,9 @@
     </row>
     <row r="28" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="10"/>
+        <v>91</v>
+      </c>
+      <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
@@ -2843,16 +3018,16 @@
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="11"/>
       <c r="T28" s="9"/>
       <c r="U28" s="9"/>
       <c r="V28" s="9"/>
@@ -2865,26 +3040,26 @@
     </row>
     <row r="29" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A29" s="13" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="11"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
       <c r="T29" s="9"/>
       <c r="U29" s="9"/>
       <c r="V29" s="9"/>
@@ -2897,26 +3072,26 @@
     </row>
     <row r="30" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A30" s="13" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="10"/>
+      <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
       <c r="T30" s="9"/>
       <c r="U30" s="9"/>
       <c r="V30" s="9"/>
@@ -2929,7 +3104,7 @@
     </row>
     <row r="31" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -2939,16 +3114,16 @@
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>
       <c r="V31" s="9"/>
@@ -2960,27 +3135,27 @@
       <c r="AB31" s="9"/>
     </row>
     <row r="32" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="10"/>
+      <c r="A32" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="11"/>
       <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
       <c r="T32" s="9"/>
       <c r="U32" s="9"/>
       <c r="V32" s="9"/>
@@ -2992,8 +3167,8 @@
       <c r="AB32" s="9"/>
     </row>
     <row r="33" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="18" t="s">
-        <v>32</v>
+      <c r="A33" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="10"/>
@@ -3003,16 +3178,16 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
       <c r="T33" s="9"/>
       <c r="U33" s="9"/>
       <c r="V33" s="9"/>
@@ -3024,27 +3199,27 @@
       <c r="AB33" s="9"/>
     </row>
     <row r="34" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="18" t="s">
-        <v>33</v>
+      <c r="A34" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="10"/>
+      <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
       <c r="T34" s="9"/>
       <c r="U34" s="9"/>
       <c r="V34" s="9"/>
@@ -3056,27 +3231,27 @@
       <c r="AB34" s="9"/>
     </row>
     <row r="35" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="18" t="s">
-        <v>34</v>
+      <c r="A35" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="10"/>
+      <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
       <c r="T35" s="9"/>
       <c r="U35" s="9"/>
       <c r="V35" s="9"/>
@@ -3088,27 +3263,27 @@
       <c r="AB35" s="9"/>
     </row>
     <row r="36" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="10"/>
+      <c r="A36" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
-      <c r="G36" s="10"/>
+      <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
       <c r="V36" s="9"/>
@@ -3120,27 +3295,27 @@
       <c r="AB36" s="9"/>
     </row>
     <row r="37" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="17" t="s">
-        <v>14</v>
+      <c r="A37" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="10"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
       <c r="T37" s="9"/>
       <c r="U37" s="9"/>
       <c r="V37" s="9"/>
@@ -3152,27 +3327,27 @@
       <c r="AB37" s="9"/>
     </row>
     <row r="38" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="11"/>
+      <c r="A38" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="10"/>
+      <c r="G38" s="11"/>
       <c r="H38" s="11"/>
       <c r="I38" s="10"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
       <c r="V38" s="9"/>
@@ -3184,27 +3359,27 @@
       <c r="AB38" s="9"/>
     </row>
     <row r="39" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="13" t="s">
-        <v>54</v>
+      <c r="A39" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
       <c r="T39" s="9"/>
       <c r="U39" s="9"/>
       <c r="V39" s="9"/>
@@ -3216,27 +3391,27 @@
       <c r="AB39" s="9"/>
     </row>
     <row r="40" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="13" t="s">
-        <v>35</v>
+      <c r="A40" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="10"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
       <c r="T40" s="9"/>
       <c r="U40" s="9"/>
       <c r="V40" s="9"/>
@@ -3248,27 +3423,27 @@
       <c r="AB40" s="9"/>
     </row>
     <row r="41" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="11"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
       <c r="T41" s="9"/>
       <c r="U41" s="9"/>
       <c r="V41" s="9"/>
@@ -3280,27 +3455,27 @@
       <c r="AB41" s="9"/>
     </row>
     <row r="42" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="13" t="s">
-        <v>36</v>
+      <c r="A42" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
       <c r="I42" s="10"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="9"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
       <c r="T42" s="9"/>
       <c r="U42" s="9"/>
       <c r="V42" s="9"/>
@@ -3312,27 +3487,27 @@
       <c r="AB42" s="9"/>
     </row>
     <row r="43" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11"/>
+      <c r="A43" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="10"/>
+      <c r="G43" s="11"/>
       <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
       <c r="T43" s="9"/>
       <c r="U43" s="9"/>
       <c r="V43" s="9"/>
@@ -3343,10 +3518,939 @@
       <c r="AA43" s="9"/>
       <c r="AB43" s="9"/>
     </row>
+    <row r="44" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A44" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
+      <c r="W44" s="9"/>
+      <c r="X44" s="9"/>
+      <c r="Y44" s="9"/>
+      <c r="Z44" s="9"/>
+      <c r="AA44" s="9"/>
+      <c r="AB44" s="9"/>
+    </row>
+    <row r="45" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="9"/>
+      <c r="U45" s="9"/>
+      <c r="V45" s="9"/>
+      <c r="W45" s="9"/>
+      <c r="X45" s="9"/>
+      <c r="Y45" s="9"/>
+      <c r="Z45" s="9"/>
+      <c r="AA45" s="9"/>
+      <c r="AB45" s="9"/>
+    </row>
+    <row r="46" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="9"/>
+      <c r="U46" s="9"/>
+      <c r="V46" s="9"/>
+      <c r="W46" s="9"/>
+      <c r="X46" s="9"/>
+      <c r="Y46" s="9"/>
+      <c r="Z46" s="9"/>
+      <c r="AA46" s="9"/>
+      <c r="AB46" s="9"/>
+    </row>
+    <row r="47" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A47" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="9"/>
+      <c r="Z47" s="9"/>
+      <c r="AA47" s="9"/>
+      <c r="AB47" s="9"/>
+    </row>
+    <row r="48" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="9"/>
+      <c r="X48" s="9"/>
+      <c r="Y48" s="9"/>
+      <c r="Z48" s="9"/>
+      <c r="AA48" s="9"/>
+      <c r="AB48" s="9"/>
+    </row>
+    <row r="49" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A49" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+      <c r="V49" s="9"/>
+      <c r="W49" s="9"/>
+      <c r="X49" s="9"/>
+      <c r="Y49" s="9"/>
+      <c r="Z49" s="9"/>
+      <c r="AA49" s="9"/>
+      <c r="AB49" s="9"/>
+    </row>
+    <row r="50" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A50" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="9"/>
+      <c r="Y50" s="9"/>
+      <c r="Z50" s="9"/>
+      <c r="AA50" s="9"/>
+      <c r="AB50" s="9"/>
+    </row>
+    <row r="51" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A51" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="9"/>
+      <c r="Z51" s="9"/>
+      <c r="AA51" s="9"/>
+      <c r="AB51" s="9"/>
+    </row>
+    <row r="52" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A52" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="9"/>
+      <c r="U52" s="9"/>
+      <c r="V52" s="9"/>
+      <c r="W52" s="9"/>
+      <c r="X52" s="9"/>
+      <c r="Y52" s="9"/>
+      <c r="Z52" s="9"/>
+      <c r="AA52" s="9"/>
+      <c r="AB52" s="9"/>
+    </row>
+    <row r="53" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="9"/>
+      <c r="V53" s="9"/>
+      <c r="W53" s="9"/>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="9"/>
+      <c r="Z53" s="9"/>
+      <c r="AA53" s="9"/>
+      <c r="AB53" s="9"/>
+    </row>
+    <row r="54" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A54" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="11"/>
+      <c r="R54" s="11"/>
+      <c r="S54" s="11"/>
+      <c r="T54" s="9"/>
+      <c r="U54" s="9"/>
+      <c r="V54" s="9"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="9"/>
+      <c r="Y54" s="9"/>
+      <c r="Z54" s="9"/>
+      <c r="AA54" s="9"/>
+      <c r="AB54" s="9"/>
+    </row>
+    <row r="55" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A55" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="11"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+      <c r="R55" s="11"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="9"/>
+      <c r="U55" s="9"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="9"/>
+      <c r="Z55" s="9"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="9"/>
+    </row>
+    <row r="56" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A56" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="9"/>
+      <c r="U56" s="9"/>
+      <c r="V56" s="9"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="9"/>
+      <c r="Z56" s="9"/>
+      <c r="AA56" s="9"/>
+      <c r="AB56" s="9"/>
+    </row>
+    <row r="57" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A57" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="9"/>
+      <c r="U57" s="9"/>
+      <c r="V57" s="9"/>
+      <c r="W57" s="9"/>
+      <c r="X57" s="9"/>
+      <c r="Y57" s="9"/>
+      <c r="Z57" s="9"/>
+      <c r="AA57" s="9"/>
+      <c r="AB57" s="9"/>
+    </row>
+    <row r="58" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A58" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="9"/>
+      <c r="U58" s="9"/>
+      <c r="V58" s="9"/>
+      <c r="W58" s="9"/>
+      <c r="X58" s="9"/>
+      <c r="Y58" s="9"/>
+      <c r="Z58" s="9"/>
+      <c r="AA58" s="9"/>
+      <c r="AB58" s="9"/>
+    </row>
+    <row r="59" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A59" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="9"/>
+      <c r="U59" s="9"/>
+      <c r="V59" s="9"/>
+      <c r="W59" s="9"/>
+      <c r="X59" s="9"/>
+      <c r="Y59" s="9"/>
+      <c r="Z59" s="9"/>
+      <c r="AA59" s="9"/>
+      <c r="AB59" s="9"/>
+    </row>
+    <row r="60" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A60" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="11"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="9"/>
+      <c r="U60" s="9"/>
+      <c r="V60" s="9"/>
+      <c r="W60" s="9"/>
+      <c r="X60" s="9"/>
+      <c r="Y60" s="9"/>
+      <c r="Z60" s="9"/>
+      <c r="AA60" s="9"/>
+      <c r="AB60" s="9"/>
+    </row>
+    <row r="61" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A61" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="11"/>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="11"/>
+      <c r="T61" s="9"/>
+      <c r="U61" s="9"/>
+      <c r="V61" s="9"/>
+      <c r="W61" s="9"/>
+      <c r="X61" s="9"/>
+      <c r="Y61" s="9"/>
+      <c r="Z61" s="9"/>
+      <c r="AA61" s="9"/>
+      <c r="AB61" s="9"/>
+    </row>
+    <row r="62" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A62" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+      <c r="O62" s="11"/>
+      <c r="P62" s="11"/>
+      <c r="Q62" s="11"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="11"/>
+      <c r="T62" s="9"/>
+      <c r="U62" s="9"/>
+      <c r="V62" s="9"/>
+      <c r="W62" s="9"/>
+      <c r="X62" s="9"/>
+      <c r="Y62" s="9"/>
+      <c r="Z62" s="9"/>
+      <c r="AA62" s="9"/>
+      <c r="AB62" s="9"/>
+    </row>
+    <row r="63" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A63" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+      <c r="N63" s="10"/>
+      <c r="O63" s="11"/>
+      <c r="P63" s="11"/>
+      <c r="Q63" s="11"/>
+      <c r="R63" s="11"/>
+      <c r="S63" s="11"/>
+      <c r="T63" s="9"/>
+      <c r="U63" s="9"/>
+      <c r="V63" s="9"/>
+      <c r="W63" s="9"/>
+      <c r="X63" s="9"/>
+      <c r="Y63" s="9"/>
+      <c r="Z63" s="9"/>
+      <c r="AA63" s="9"/>
+      <c r="AB63" s="9"/>
+    </row>
+    <row r="64" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="T64" s="9"/>
+      <c r="U64" s="9"/>
+      <c r="V64" s="9"/>
+      <c r="W64" s="9"/>
+      <c r="X64" s="9"/>
+      <c r="Y64" s="9"/>
+      <c r="Z64" s="9"/>
+      <c r="AA64" s="9"/>
+      <c r="AB64" s="9"/>
+    </row>
+    <row r="65" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A65" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11"/>
+      <c r="O65" s="11"/>
+      <c r="P65" s="11"/>
+      <c r="Q65" s="11"/>
+      <c r="R65" s="11"/>
+      <c r="S65" s="11"/>
+      <c r="T65" s="9"/>
+      <c r="U65" s="9"/>
+      <c r="V65" s="9"/>
+      <c r="W65" s="9"/>
+      <c r="X65" s="9"/>
+      <c r="Y65" s="9"/>
+      <c r="Z65" s="9"/>
+      <c r="AA65" s="9"/>
+      <c r="AB65" s="9"/>
+    </row>
+    <row r="66" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A66" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="11"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
+      <c r="T66" s="9"/>
+      <c r="U66" s="9"/>
+      <c r="V66" s="9"/>
+      <c r="W66" s="9"/>
+      <c r="X66" s="9"/>
+      <c r="Y66" s="9"/>
+      <c r="Z66" s="9"/>
+      <c r="AA66" s="9"/>
+      <c r="AB66" s="9"/>
+    </row>
+    <row r="67" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A67" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+      <c r="P67" s="11"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="11"/>
+      <c r="S67" s="11"/>
+      <c r="T67" s="9"/>
+      <c r="U67" s="9"/>
+      <c r="V67" s="9"/>
+      <c r="W67" s="9"/>
+      <c r="X67" s="9"/>
+      <c r="Y67" s="9"/>
+      <c r="Z67" s="9"/>
+      <c r="AA67" s="9"/>
+      <c r="AB67" s="9"/>
+    </row>
+    <row r="68" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A68" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="11"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="11"/>
+      <c r="O68" s="11"/>
+      <c r="P68" s="11"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="11"/>
+      <c r="S68" s="11"/>
+      <c r="T68" s="9"/>
+      <c r="U68" s="9"/>
+      <c r="V68" s="9"/>
+      <c r="W68" s="9"/>
+      <c r="X68" s="9"/>
+      <c r="Y68" s="9"/>
+      <c r="Z68" s="9"/>
+      <c r="AA68" s="9"/>
+      <c r="AB68" s="9"/>
+    </row>
+    <row r="69" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A69" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="11"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="11"/>
+      <c r="T69" s="9"/>
+      <c r="U69" s="9"/>
+      <c r="V69" s="9"/>
+      <c r="W69" s="9"/>
+      <c r="X69" s="9"/>
+      <c r="Y69" s="9"/>
+      <c r="Z69" s="9"/>
+      <c r="AA69" s="9"/>
+      <c r="AB69" s="9"/>
+    </row>
+    <row r="70" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A70" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11"/>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+      <c r="P70" s="11"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="11"/>
+      <c r="S70" s="11"/>
+      <c r="T70" s="9"/>
+      <c r="U70" s="9"/>
+      <c r="V70" s="9"/>
+      <c r="W70" s="9"/>
+      <c r="X70" s="9"/>
+      <c r="Y70" s="9"/>
+      <c r="Z70" s="9"/>
+      <c r="AA70" s="9"/>
+      <c r="AB70" s="9"/>
+    </row>
+    <row r="71" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A71" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="10"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
+      <c r="T71" s="9"/>
+      <c r="U71" s="9"/>
+      <c r="V71" s="9"/>
+      <c r="W71" s="9"/>
+      <c r="X71" s="9"/>
+      <c r="Y71" s="9"/>
+      <c r="Z71" s="9"/>
+      <c r="AA71" s="9"/>
+      <c r="AB71" s="9"/>
+    </row>
+    <row r="72" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A72" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="11"/>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+      <c r="N72" s="11"/>
+      <c r="O72" s="11"/>
+      <c r="P72" s="11"/>
+      <c r="Q72" s="10"/>
+      <c r="R72" s="11"/>
+      <c r="S72" s="11"/>
+      <c r="T72" s="9"/>
+      <c r="U72" s="9"/>
+      <c r="V72" s="9"/>
+      <c r="W72" s="9"/>
+      <c r="X72" s="9"/>
+      <c r="Y72" s="9"/>
+      <c r="Z72" s="9"/>
+      <c r="AA72" s="9"/>
+      <c r="AB72" s="9"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I43" xr:uid="{789F7D5E-0CCD-4167-8637-C613F47B1A4E}"/>
+  <autoFilter ref="A1:S72" xr:uid="{BF2C8562-5E79-4762-A239-ADC991581BA9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added ComboBox to Header Panel
Put ComboBox for Manufacturer and Model. Also installed Prism for DelegateCommand for button. Added Submitted button.
</commit_message>
<xml_diff>
--- a/ScheduleEntryForms/Documentation/DataFieldMatrix.xlsx
+++ b/ScheduleEntryForms/Documentation/DataFieldMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhanp\source\repos\nhanphan2112\Aire.DataEntryForms\ScheduleEntryForms\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CE7FBA-E816-4A97-AF0D-38839B1F610F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDEDDB1-D57F-4CEA-8062-0C64954E5379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B54BB1EA-0F42-48C7-90BB-C62F55C48395}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B54BB1EA-0F42-48C7-90BB-C62F55C48395}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2095,11 +2095,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D3163-F64C-485F-B08A-A467FA0F7EED}">
   <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U1" sqref="U1"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added Electrical Configuration Property to the ElectricalConfigurationPanelViewModel
The ElectricalConfiguration eliminate the needs for local boolean properties used to control visibility in the view. XAML visibility can now bind directly to fields in the ElectricalConfiguration.
</commit_message>
<xml_diff>
--- a/ScheduleEntryForms/Documentation/DataFieldMatrix.xlsx
+++ b/ScheduleEntryForms/Documentation/DataFieldMatrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhanp\source\repos\nhanphan2112\Aire.DataEntryForms\ScheduleEntryForms\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDEDDB1-D57F-4CEA-8062-0C64954E5379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B83C11-B011-4EC6-AC5B-F3C64A783CA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B54BB1EA-0F42-48C7-90BB-C62F55C48395}"/>
   </bookViews>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -643,7 +643,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
@@ -2095,11 +2094,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D3163-F64C-485F-B08A-A467FA0F7EED}">
   <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomRight" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2271,7 +2270,7 @@
       <c r="AB4" s="9"/>
     </row>
     <row r="5" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="11"/>
@@ -2303,7 +2302,7 @@
       <c r="AB5" s="9"/>
     </row>
     <row r="6" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="11"/>
@@ -3551,7 +3550,7 @@
       <c r="AB44" s="9"/>
     </row>
     <row r="45" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B45" s="11"/>
@@ -3583,7 +3582,7 @@
       <c r="AB45" s="9"/>
     </row>
     <row r="46" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B46" s="10"/>

</xml_diff>